<commit_message>
keep Q&A as list
</commit_message>
<xml_diff>
--- a/MRTuser.xlsx
+++ b/MRTuser.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Datast\datast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FA03F6-E863-42D3-8469-FE17314847CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE56E24-1466-416C-9F2C-D656C91A46DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
     <author>Admin</author>
   </authors>
   <commentList>
-    <comment ref="E30" authorId="0" shapeId="0" xr:uid="{3CD0F3CB-835A-4EB6-B8F7-B4C3AFFB23B2}">
+    <comment ref="E31" authorId="0" shapeId="0" xr:uid="{3CD0F3CB-835A-4EB6-B8F7-B4C3AFFB23B2}">
       <text>
         <r>
           <rPr>
@@ -61,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E31" authorId="0" shapeId="0" xr:uid="{2CE7D8D8-2731-491C-8630-54A1ECE85823}">
+    <comment ref="E32" authorId="0" shapeId="0" xr:uid="{2CE7D8D8-2731-491C-8630-54A1ECE85823}">
       <text>
         <r>
           <rPr>
@@ -85,7 +85,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G32" authorId="0" shapeId="0" xr:uid="{6E761427-24A1-4AAD-B8FE-18B3819CB7BD}">
+    <comment ref="G33" authorId="0" shapeId="0" xr:uid="{6E761427-24A1-4AAD-B8FE-18B3819CB7BD}">
       <text>
         <r>
           <rPr>
@@ -109,7 +109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E34" authorId="0" shapeId="0" xr:uid="{ABE28B14-8AFD-4D5F-BDFD-AFF40BD64FF6}">
+    <comment ref="E35" authorId="0" shapeId="0" xr:uid="{ABE28B14-8AFD-4D5F-BDFD-AFF40BD64FF6}">
       <text>
         <r>
           <rPr>
@@ -133,7 +133,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{FD038423-1508-485A-A9A0-D5B102B0309C}">
+    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{FD038423-1508-485A-A9A0-D5B102B0309C}">
       <text>
         <r>
           <rPr>
@@ -157,7 +157,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G34" authorId="0" shapeId="0" xr:uid="{B1BDC5A7-8805-4A2F-B6A2-A77CDE91961D}">
+    <comment ref="G35" authorId="0" shapeId="0" xr:uid="{B1BDC5A7-8805-4A2F-B6A2-A77CDE91961D}">
       <text>
         <r>
           <rPr>
@@ -181,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E43" authorId="0" shapeId="0" xr:uid="{705CCF46-F1C5-439E-8CF5-1166632BFD9B}">
+    <comment ref="E44" authorId="0" shapeId="0" xr:uid="{705CCF46-F1C5-439E-8CF5-1166632BFD9B}">
       <text>
         <r>
           <rPr>
@@ -210,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="55">
   <si>
     <t>เดือน</t>
   </si>
@@ -1158,15 +1158,15 @@
   <dimension ref="A1:G138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" x14ac:dyDescent="0.65"/>
   <cols>
     <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.19921875" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.69921875" style="1" customWidth="1"/>
     <col min="5" max="5" width="21.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27" style="1" bestFit="1" customWidth="1"/>
@@ -3144,40 +3144,48 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12E07C45-672B-49A2-B9A9-DF84CE32B973}">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="4.8984375" customWidth="1"/>
+    <col min="3" max="3" width="32.59765625" customWidth="1"/>
+    <col min="4" max="4" width="17.09765625" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="28.69921875" customWidth="1"/>
+    <col min="7" max="7" width="26.09765625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.65">
-      <c r="A1" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="15">
-        <v>2559</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="19">
-        <v>532026</v>
-      </c>
-      <c r="E1" s="19">
-        <v>20172</v>
-      </c>
-      <c r="F1" s="21">
-        <v>20492</v>
-      </c>
-      <c r="G1" s="20">
-        <v>19568</v>
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A2" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="15">
         <v>2559</v>
@@ -3186,21 +3194,21 @@
         <v>54</v>
       </c>
       <c r="D2" s="19">
-        <v>629963</v>
+        <v>532026</v>
       </c>
       <c r="E2" s="19">
-        <v>20999</v>
+        <v>20172</v>
       </c>
       <c r="F2" s="21">
-        <v>22658</v>
+        <v>20492</v>
       </c>
       <c r="G2" s="20">
-        <v>16437</v>
+        <v>19568</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A3" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="15">
         <v>2559</v>
@@ -3208,22 +3216,22 @@
       <c r="C3" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="20">
-        <v>650772</v>
+      <c r="D3" s="19">
+        <v>629963</v>
       </c>
       <c r="E3" s="19">
-        <v>20993</v>
+        <v>20999</v>
       </c>
       <c r="F3" s="21">
-        <v>24212</v>
+        <v>22658</v>
       </c>
       <c r="G3" s="20">
-        <v>15140</v>
+        <v>16437</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A4" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="15">
         <v>2559</v>
@@ -3232,21 +3240,21 @@
         <v>54</v>
       </c>
       <c r="D4" s="20">
-        <v>647337</v>
+        <v>650772</v>
       </c>
       <c r="E4" s="19">
-        <v>21578</v>
+        <v>20993</v>
       </c>
       <c r="F4" s="21">
-        <v>24238</v>
+        <v>24212</v>
       </c>
       <c r="G4" s="20">
-        <v>14264</v>
+        <v>15140</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A5" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="15">
         <v>2559</v>
@@ -3255,44 +3263,44 @@
         <v>54</v>
       </c>
       <c r="D5" s="20">
-        <v>614216</v>
+        <v>647337</v>
       </c>
       <c r="E5" s="19">
-        <v>19161</v>
+        <v>21578</v>
       </c>
       <c r="F5" s="21">
-        <v>23048</v>
+        <v>24238</v>
       </c>
       <c r="G5" s="20">
-        <v>12093</v>
+        <v>14264</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A6" s="15" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B6" s="15">
-        <v>2560</v>
+        <v>2559</v>
       </c>
       <c r="C6" s="23" t="s">
         <v>54</v>
       </c>
       <c r="D6" s="20">
-        <v>637589</v>
+        <v>614216</v>
       </c>
       <c r="E6" s="19">
-        <v>20500</v>
+        <v>19161</v>
       </c>
       <c r="F6" s="21">
-        <v>24330</v>
-      </c>
-      <c r="G6" s="22">
-        <v>13538</v>
+        <v>23048</v>
+      </c>
+      <c r="G6" s="20">
+        <v>12093</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A7" s="15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="15">
         <v>2560</v>
@@ -3301,21 +3309,21 @@
         <v>54</v>
       </c>
       <c r="D7" s="20">
-        <v>610955</v>
+        <v>637589</v>
       </c>
       <c r="E7" s="19">
-        <v>21822</v>
+        <v>20500</v>
       </c>
       <c r="F7" s="21">
-        <v>25410</v>
+        <v>24330</v>
       </c>
       <c r="G7" s="22">
-        <v>14248</v>
+        <v>13538</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A8" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="15">
         <v>2560</v>
@@ -3324,21 +3332,21 @@
         <v>54</v>
       </c>
       <c r="D8" s="20">
-        <v>719225</v>
+        <v>610955</v>
       </c>
       <c r="E8" s="19">
-        <v>23201</v>
+        <v>21822</v>
       </c>
       <c r="F8" s="21">
-        <v>25447</v>
+        <v>25410</v>
       </c>
       <c r="G8" s="22">
-        <v>16741</v>
+        <v>14248</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A9" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="15">
         <v>2560</v>
@@ -3347,21 +3355,21 @@
         <v>54</v>
       </c>
       <c r="D9" s="20">
-        <v>631343</v>
+        <v>719225</v>
       </c>
       <c r="E9" s="19">
-        <v>21045</v>
+        <v>23201</v>
       </c>
       <c r="F9" s="21">
-        <v>25678</v>
+        <v>25447</v>
       </c>
       <c r="G9" s="22">
-        <v>15750</v>
+        <v>16741</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A10" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="15">
         <v>2560</v>
@@ -3370,21 +3378,21 @@
         <v>54</v>
       </c>
       <c r="D10" s="20">
-        <v>747530</v>
+        <v>631343</v>
       </c>
       <c r="E10" s="19">
-        <v>24144</v>
+        <v>21045</v>
       </c>
       <c r="F10" s="21">
-        <v>28127</v>
+        <v>25678</v>
       </c>
       <c r="G10" s="22">
-        <v>16901</v>
+        <v>15750</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A11" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B11" s="15">
         <v>2560</v>
@@ -3393,21 +3401,21 @@
         <v>54</v>
       </c>
       <c r="D11" s="20">
-        <v>817146</v>
+        <v>747530</v>
       </c>
       <c r="E11" s="19">
-        <v>27243</v>
+        <v>24144</v>
       </c>
       <c r="F11" s="21">
-        <v>30217</v>
+        <v>28127</v>
       </c>
       <c r="G11" s="22">
-        <v>19066</v>
+        <v>16901</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A12" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="15">
         <v>2560</v>
@@ -3416,21 +3424,21 @@
         <v>54</v>
       </c>
       <c r="D12" s="20">
-        <v>812445</v>
+        <v>817146</v>
       </c>
       <c r="E12" s="19">
-        <v>26565</v>
+        <v>27243</v>
       </c>
       <c r="F12" s="21">
-        <v>31501</v>
+        <v>30217</v>
       </c>
       <c r="G12" s="22">
-        <v>18749</v>
+        <v>19066</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A13" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="15">
         <v>2560</v>
@@ -3439,21 +3447,21 @@
         <v>54</v>
       </c>
       <c r="D13" s="20">
-        <v>1308446</v>
+        <v>812445</v>
       </c>
       <c r="E13" s="19">
-        <v>38931</v>
+        <v>26565</v>
       </c>
       <c r="F13" s="21">
-        <v>43224</v>
+        <v>31501</v>
       </c>
       <c r="G13" s="22">
-        <v>28436</v>
+        <v>18749</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A14" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="15">
         <v>2560</v>
@@ -3462,21 +3470,21 @@
         <v>54</v>
       </c>
       <c r="D14" s="20">
-        <v>1622195</v>
+        <v>1308446</v>
       </c>
       <c r="E14" s="19">
-        <v>46909</v>
+        <v>38931</v>
       </c>
       <c r="F14" s="21">
-        <v>52322</v>
+        <v>43224</v>
       </c>
       <c r="G14" s="22">
-        <v>34278</v>
+        <v>28436</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A15" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="15">
         <v>2560</v>
@@ -3485,21 +3493,21 @@
         <v>54</v>
       </c>
       <c r="D15" s="20">
-        <v>1390911</v>
+        <v>1622195</v>
       </c>
       <c r="E15" s="19">
-        <v>45897</v>
+        <v>46909</v>
       </c>
       <c r="F15" s="21">
-        <v>53861</v>
+        <v>52322</v>
       </c>
       <c r="G15" s="22">
-        <v>32140</v>
+        <v>34278</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A16" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="15">
         <v>2560</v>
@@ -3508,21 +3516,21 @@
         <v>54</v>
       </c>
       <c r="D16" s="20">
-        <v>1394867</v>
+        <v>1390911</v>
       </c>
       <c r="E16" s="19">
-        <v>46519</v>
+        <v>45897</v>
       </c>
       <c r="F16" s="21">
-        <v>52042</v>
+        <v>53861</v>
       </c>
       <c r="G16" s="22">
-        <v>31330</v>
+        <v>32140</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A17" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="15">
         <v>2560</v>
@@ -3531,44 +3539,44 @@
         <v>54</v>
       </c>
       <c r="D17" s="20">
-        <v>1178015</v>
+        <v>1394867</v>
       </c>
       <c r="E17" s="19">
-        <v>40311</v>
+        <v>46519</v>
       </c>
       <c r="F17" s="21">
-        <v>48421</v>
+        <v>52042</v>
       </c>
       <c r="G17" s="22">
-        <v>27470</v>
+        <v>31330</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A18" s="15" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B18" s="15">
-        <v>2561</v>
+        <v>2560</v>
       </c>
       <c r="C18" s="23" t="s">
         <v>54</v>
       </c>
       <c r="D18" s="20">
-        <v>1265194</v>
+        <v>1178015</v>
       </c>
       <c r="E18" s="19">
-        <v>42748</v>
+        <v>40311</v>
       </c>
       <c r="F18" s="21">
-        <v>50011</v>
+        <v>48421</v>
       </c>
       <c r="G18" s="22">
-        <v>27495</v>
+        <v>27470</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A19" s="15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19" s="15">
         <v>2561</v>
@@ -3577,21 +3585,21 @@
         <v>54</v>
       </c>
       <c r="D19" s="20">
-        <v>1245391</v>
+        <v>1265194</v>
       </c>
       <c r="E19" s="19">
-        <v>45228</v>
+        <v>42748</v>
       </c>
       <c r="F19" s="21">
-        <v>51381</v>
+        <v>50011</v>
       </c>
       <c r="G19" s="22">
-        <v>29846</v>
+        <v>27495</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A20" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" s="15">
         <v>2561</v>
@@ -3600,21 +3608,21 @@
         <v>54</v>
       </c>
       <c r="D20" s="20">
-        <v>1373053</v>
+        <v>1245391</v>
       </c>
       <c r="E20" s="19">
-        <v>45004</v>
+        <v>45228</v>
       </c>
       <c r="F20" s="21">
-        <v>51731</v>
+        <v>51381</v>
       </c>
       <c r="G20" s="22">
-        <v>30877</v>
+        <v>29846</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A21" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" s="15">
         <v>2561</v>
@@ -3623,21 +3631,21 @@
         <v>54</v>
       </c>
       <c r="D21" s="20">
-        <v>1222331</v>
+        <v>1373053</v>
       </c>
       <c r="E21" s="19">
-        <v>40833</v>
+        <v>45004</v>
       </c>
       <c r="F21" s="21">
-        <v>51597</v>
+        <v>51731</v>
       </c>
       <c r="G21" s="22">
-        <v>26756</v>
+        <v>30877</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A22" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" s="15">
         <v>2561</v>
@@ -3646,21 +3654,21 @@
         <v>54</v>
       </c>
       <c r="D22" s="20">
-        <v>1373252</v>
+        <v>1222331</v>
       </c>
       <c r="E22" s="19">
-        <v>45050</v>
+        <v>40833</v>
       </c>
       <c r="F22" s="21">
-        <v>53101</v>
+        <v>51597</v>
       </c>
       <c r="G22" s="22">
-        <v>30412</v>
+        <v>26756</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A23" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B23" s="15">
         <v>2561</v>
@@ -3669,21 +3677,21 @@
         <v>54</v>
       </c>
       <c r="D23" s="20">
-        <v>1504118</v>
+        <v>1373252</v>
       </c>
       <c r="E23" s="19">
-        <v>49964</v>
+        <v>45050</v>
       </c>
       <c r="F23" s="21">
-        <v>57088</v>
+        <v>53101</v>
       </c>
       <c r="G23" s="22">
-        <v>33341</v>
+        <v>30412</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A24" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" s="15">
         <v>2561</v>
@@ -3692,21 +3700,21 @@
         <v>54</v>
       </c>
       <c r="D24" s="20">
-        <v>1466777</v>
+        <v>1504118</v>
       </c>
       <c r="E24" s="19">
-        <v>48613</v>
+        <v>49964</v>
       </c>
       <c r="F24" s="21">
-        <v>58741</v>
+        <v>57088</v>
       </c>
       <c r="G24" s="22">
-        <v>30199</v>
+        <v>33341</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A25" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" s="15">
         <v>2561</v>
@@ -3715,21 +3723,21 @@
         <v>54</v>
       </c>
       <c r="D25" s="20">
-        <v>1683823</v>
+        <v>1466777</v>
       </c>
       <c r="E25" s="19">
-        <v>54223</v>
+        <v>48613</v>
       </c>
       <c r="F25" s="21">
-        <v>62892</v>
+        <v>58741</v>
       </c>
       <c r="G25" s="22">
-        <v>33034</v>
+        <v>30199</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A26" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B26" s="15">
         <v>2561</v>
@@ -3738,21 +3746,21 @@
         <v>54</v>
       </c>
       <c r="D26" s="20">
-        <v>1585030</v>
+        <v>1683823</v>
       </c>
       <c r="E26" s="19">
-        <v>53453</v>
+        <v>54223</v>
       </c>
       <c r="F26" s="21">
-        <v>62352</v>
+        <v>62892</v>
       </c>
       <c r="G26" s="22">
-        <v>35653</v>
+        <v>33034</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A27" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27" s="15">
         <v>2561</v>
@@ -3761,21 +3769,21 @@
         <v>54</v>
       </c>
       <c r="D27" s="20">
-        <v>1565132</v>
+        <v>1585030</v>
       </c>
       <c r="E27" s="19">
-        <v>51304</v>
+        <v>53453</v>
       </c>
       <c r="F27" s="21">
-        <v>60299</v>
+        <v>62352</v>
       </c>
       <c r="G27" s="22">
-        <v>32414</v>
+        <v>35653</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A28" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" s="15">
         <v>2561</v>
@@ -3784,21 +3792,21 @@
         <v>54</v>
       </c>
       <c r="D28" s="20">
-        <v>1646422</v>
+        <v>1565132</v>
       </c>
       <c r="E28" s="19">
-        <v>55070</v>
+        <v>51304</v>
       </c>
       <c r="F28" s="21">
-        <v>62003</v>
+        <v>60299</v>
       </c>
       <c r="G28" s="22">
-        <v>36004</v>
+        <v>32414</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A29" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B29" s="15">
         <v>2561</v>
@@ -3807,44 +3815,44 @@
         <v>54</v>
       </c>
       <c r="D29" s="20">
-        <v>1478857</v>
+        <v>1646422</v>
       </c>
       <c r="E29" s="19">
-        <v>47859</v>
+        <v>55070</v>
       </c>
       <c r="F29" s="21">
-        <v>58140</v>
+        <v>62003</v>
       </c>
       <c r="G29" s="22">
-        <v>33624</v>
+        <v>36004</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A30" s="15" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B30" s="15">
-        <v>2562</v>
+        <v>2561</v>
       </c>
       <c r="C30" s="23" t="s">
         <v>54</v>
       </c>
       <c r="D30" s="20">
-        <v>1587555</v>
+        <v>1478857</v>
       </c>
       <c r="E30" s="19">
-        <v>51347</v>
+        <v>47859</v>
       </c>
       <c r="F30" s="21">
-        <v>59159</v>
+        <v>58140</v>
       </c>
       <c r="G30" s="22">
-        <v>32252</v>
+        <v>33624</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A31" s="15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B31" s="15">
         <v>2562</v>
@@ -3853,21 +3861,21 @@
         <v>54</v>
       </c>
       <c r="D31" s="20">
-        <v>1391757</v>
+        <v>1587555</v>
       </c>
       <c r="E31" s="19">
-        <v>51548</v>
+        <v>51347</v>
       </c>
       <c r="F31" s="21">
-        <v>60349</v>
+        <v>59159</v>
       </c>
       <c r="G31" s="22">
-        <v>32967</v>
+        <v>32252</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A32" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B32" s="15">
         <v>2562</v>
@@ -3876,21 +3884,21 @@
         <v>54</v>
       </c>
       <c r="D32" s="20">
-        <v>1651391</v>
+        <v>1391757</v>
       </c>
       <c r="E32" s="19">
-        <v>53701</v>
+        <v>51548</v>
       </c>
       <c r="F32" s="21">
-        <v>61262</v>
+        <v>60349</v>
       </c>
       <c r="G32" s="22">
-        <v>37284</v>
+        <v>32967</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A33" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B33" s="15">
         <v>2562</v>
@@ -3899,21 +3907,21 @@
         <v>54</v>
       </c>
       <c r="D33" s="20">
-        <v>1448402</v>
+        <v>1651391</v>
       </c>
       <c r="E33" s="19">
-        <v>48630</v>
+        <v>53701</v>
       </c>
       <c r="F33" s="21">
-        <v>61016</v>
+        <v>61262</v>
       </c>
       <c r="G33" s="22">
-        <v>30052</v>
+        <v>37284</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A34" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B34" s="15">
         <v>2562</v>
@@ -3922,21 +3930,21 @@
         <v>54</v>
       </c>
       <c r="D34" s="20">
-        <v>1598725</v>
+        <v>1448402</v>
       </c>
       <c r="E34" s="19">
-        <v>52790</v>
+        <v>48630</v>
       </c>
       <c r="F34" s="21">
-        <v>62586</v>
+        <v>61016</v>
       </c>
       <c r="G34" s="22">
-        <v>34177</v>
+        <v>30052</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A35" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B35" s="15">
         <v>2562</v>
@@ -3945,21 +3953,21 @@
         <v>54</v>
       </c>
       <c r="D35" s="20">
-        <v>1670264</v>
+        <v>1598725</v>
       </c>
       <c r="E35" s="19">
-        <v>55847</v>
+        <v>52790</v>
       </c>
       <c r="F35" s="21">
-        <v>67272</v>
+        <v>62586</v>
       </c>
       <c r="G35" s="22">
-        <v>36112</v>
+        <v>34177</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A36" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B36" s="15">
         <v>2562</v>
@@ -3968,21 +3976,21 @@
         <v>54</v>
       </c>
       <c r="D36" s="20">
-        <v>1745728</v>
+        <v>1670264</v>
       </c>
       <c r="E36" s="19">
-        <v>56313</v>
+        <v>55847</v>
       </c>
       <c r="F36" s="21">
-        <v>67705</v>
+        <v>67272</v>
       </c>
       <c r="G36" s="22">
-        <v>35601</v>
+        <v>36112</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A37" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B37" s="15">
         <v>2562</v>
@@ -3991,21 +3999,21 @@
         <v>54</v>
       </c>
       <c r="D37" s="20">
-        <v>1796738</v>
+        <v>1745728</v>
       </c>
       <c r="E37" s="19">
-        <v>58360</v>
+        <v>56313</v>
       </c>
       <c r="F37" s="21">
-        <v>68989</v>
+        <v>67705</v>
       </c>
       <c r="G37" s="22">
-        <v>36039</v>
+        <v>35601</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A38" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B38" s="15">
         <v>2562</v>
@@ -4014,21 +4022,21 @@
         <v>54</v>
       </c>
       <c r="D38" s="20">
-        <v>1706450</v>
+        <v>1796738</v>
       </c>
       <c r="E38" s="19">
-        <v>58104</v>
+        <v>58360</v>
       </c>
       <c r="F38" s="21">
-        <v>67377</v>
+        <v>68989</v>
       </c>
       <c r="G38" s="22">
-        <v>36468</v>
+        <v>36039</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A39" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B39" s="15">
         <v>2562</v>
@@ -4037,21 +4045,21 @@
         <v>54</v>
       </c>
       <c r="D39" s="20">
-        <v>1725517</v>
+        <v>1706450</v>
       </c>
       <c r="E39" s="19">
-        <v>55797</v>
+        <v>58104</v>
       </c>
       <c r="F39" s="21">
-        <v>65407</v>
+        <v>67377</v>
       </c>
       <c r="G39" s="22">
-        <v>35614</v>
+        <v>36468</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A40" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B40" s="15">
         <v>2562</v>
@@ -4060,21 +4068,21 @@
         <v>54</v>
       </c>
       <c r="D40" s="20">
-        <v>1752391</v>
+        <v>1725517</v>
       </c>
       <c r="E40" s="19">
-        <v>58513</v>
+        <v>55797</v>
       </c>
       <c r="F40" s="21">
-        <v>67547</v>
+        <v>65407</v>
       </c>
       <c r="G40" s="22">
-        <v>42910</v>
+        <v>35614</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A41" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B41" s="15">
         <v>2562</v>
@@ -4083,44 +4091,44 @@
         <v>54</v>
       </c>
       <c r="D41" s="20">
-        <v>1768983</v>
+        <v>1752391</v>
       </c>
       <c r="E41" s="19">
-        <v>52490</v>
+        <v>58513</v>
       </c>
       <c r="F41" s="21">
-        <v>65266</v>
+        <v>67547</v>
       </c>
       <c r="G41" s="22">
-        <v>35783</v>
+        <v>42910</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A42" s="15" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B42" s="15">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="C42" s="23" t="s">
         <v>54</v>
       </c>
       <c r="D42" s="20">
-        <v>1825447</v>
+        <v>1768983</v>
       </c>
       <c r="E42" s="19">
-        <v>58961</v>
+        <v>52490</v>
       </c>
       <c r="F42" s="21">
-        <v>67781</v>
+        <v>65266</v>
       </c>
       <c r="G42" s="22">
-        <v>37401</v>
+        <v>35783</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A43" s="15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B43" s="15">
         <v>2563</v>
@@ -4129,21 +4137,21 @@
         <v>54</v>
       </c>
       <c r="D43" s="20">
-        <v>1683249</v>
+        <v>1825447</v>
       </c>
       <c r="E43" s="19">
-        <v>57384</v>
+        <v>58961</v>
       </c>
       <c r="F43" s="21">
-        <v>68406</v>
+        <v>67781</v>
       </c>
       <c r="G43" s="22">
-        <v>36442</v>
+        <v>37401</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A44" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B44" s="15">
         <v>2563</v>
@@ -4152,21 +4160,21 @@
         <v>54</v>
       </c>
       <c r="D44" s="20">
-        <v>1219614</v>
+        <v>1683249</v>
       </c>
       <c r="E44" s="19">
-        <v>39601</v>
+        <v>57384</v>
       </c>
       <c r="F44" s="21">
-        <v>47436</v>
+        <v>68406</v>
       </c>
       <c r="G44" s="22">
-        <v>20450</v>
+        <v>36442</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A45" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B45" s="15">
         <v>2563</v>
@@ -4175,21 +4183,21 @@
         <v>54</v>
       </c>
       <c r="D45" s="20">
-        <v>438995</v>
+        <v>1219614</v>
       </c>
       <c r="E45" s="19">
-        <v>14640</v>
+        <v>39601</v>
       </c>
       <c r="F45" s="21">
-        <v>18001</v>
+        <v>47436</v>
       </c>
       <c r="G45" s="22">
-        <v>6797</v>
+        <v>20450</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A46" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B46" s="15">
         <v>2563</v>
@@ -4198,44 +4206,44 @@
         <v>54</v>
       </c>
       <c r="D46" s="20">
-        <v>674459</v>
+        <v>438995</v>
       </c>
       <c r="E46" s="19">
-        <v>21758</v>
+        <v>14640</v>
       </c>
       <c r="F46" s="21">
-        <v>28009</v>
+        <v>18001</v>
       </c>
       <c r="G46" s="22">
-        <v>14167</v>
+        <v>6797</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A47" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B47" s="15">
         <v>2563</v>
       </c>
-      <c r="C47" s="18" t="s">
+      <c r="C47" s="23" t="s">
         <v>54</v>
       </c>
       <c r="D47" s="20">
-        <v>1094312</v>
+        <v>674459</v>
       </c>
       <c r="E47" s="19">
-        <v>36477</v>
+        <v>21758</v>
       </c>
       <c r="F47" s="21">
-        <v>41687</v>
+        <v>28009</v>
       </c>
       <c r="G47" s="22">
-        <v>24320</v>
+        <v>14167</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A48" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B48" s="15">
         <v>2563</v>
@@ -4244,21 +4252,21 @@
         <v>54</v>
       </c>
       <c r="D48" s="20">
-        <v>1442882</v>
+        <v>1094312</v>
       </c>
       <c r="E48" s="19">
-        <v>57069</v>
+        <v>36477</v>
       </c>
       <c r="F48" s="21">
-        <v>46545</v>
+        <v>41687</v>
       </c>
       <c r="G48" s="22">
-        <v>29882</v>
+        <v>24320</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A49" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B49" s="15">
         <v>2563</v>
@@ -4267,21 +4275,21 @@
         <v>54</v>
       </c>
       <c r="D49" s="20">
-        <v>1643577</v>
+        <v>1442882</v>
       </c>
       <c r="E49" s="19">
-        <v>53019</v>
+        <v>57069</v>
       </c>
       <c r="F49" s="21">
-        <v>63799</v>
+        <v>46545</v>
       </c>
       <c r="G49" s="22">
-        <v>33419</v>
+        <v>29882</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A50" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B50" s="15">
         <v>2563</v>
@@ -4290,21 +4298,21 @@
         <v>54</v>
       </c>
       <c r="D50" s="20">
-        <v>1754350</v>
+        <v>1643577</v>
       </c>
       <c r="E50" s="19">
-        <v>58478</v>
+        <v>53019</v>
       </c>
       <c r="F50" s="21">
-        <v>70104</v>
+        <v>63799</v>
       </c>
       <c r="G50" s="22">
-        <v>35228</v>
+        <v>33419</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A51" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B51" s="15">
         <v>2563</v>
@@ -4313,44 +4321,44 @@
         <v>54</v>
       </c>
       <c r="D51" s="20">
+        <v>1754350</v>
+      </c>
+      <c r="E51" s="19">
+        <v>58478</v>
+      </c>
+      <c r="F51" s="21">
+        <v>70104</v>
+      </c>
+      <c r="G51" s="22">
+        <v>35228</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+      <c r="A52" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52" s="15">
+        <v>2563</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D52" s="20">
         <v>1759392</v>
       </c>
-      <c r="E51" s="19">
+      <c r="E52" s="19">
         <v>56755</v>
       </c>
-      <c r="F51" s="21">
+      <c r="F52" s="21">
         <v>69885</v>
       </c>
-      <c r="G51" s="22">
+      <c r="G52" s="22">
         <v>32882</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="24" x14ac:dyDescent="0.65">
-      <c r="A52" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B52" s="24">
-        <v>2563</v>
-      </c>
-      <c r="C52" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="D52" s="28">
-        <v>1745557</v>
-      </c>
-      <c r="E52" s="29">
-        <v>58185</v>
-      </c>
-      <c r="F52" s="30">
-        <v>68739</v>
-      </c>
-      <c r="G52" s="31">
-        <v>39956</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="24" x14ac:dyDescent="0.65">
       <c r="A53" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B53" s="24">
         <v>2563</v>
@@ -4359,15 +4367,38 @@
         <v>54</v>
       </c>
       <c r="D53" s="28">
+        <v>1745557</v>
+      </c>
+      <c r="E53" s="29">
+        <v>58185</v>
+      </c>
+      <c r="F53" s="30">
+        <v>68739</v>
+      </c>
+      <c r="G53" s="31">
+        <v>39956</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+      <c r="A54" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B54" s="24">
+        <v>2563</v>
+      </c>
+      <c r="C54" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D54" s="28">
         <v>1563252</v>
       </c>
-      <c r="E53" s="29">
+      <c r="E54" s="29">
         <v>50427</v>
       </c>
-      <c r="F53" s="30">
+      <c r="F54" s="30">
         <v>60659</v>
       </c>
-      <c r="G53" s="31">
+      <c r="G54" s="31">
         <v>31825</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Delete unique dataframe and id in function cleanDF
</commit_message>
<xml_diff>
--- a/MRTuser.xlsx
+++ b/MRTuser.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Datast\datast\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\World\Documents\SeniorProject\datast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE56E24-1466-416C-9F2C-D656C91A46DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704528B7-2FA1-4A87-AB96-89E5C8264991}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta Data" sheetId="5" r:id="rId1"/>
@@ -384,14 +384,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="187" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -399,7 +399,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -421,7 +421,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -510,7 +510,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="33">
@@ -550,23 +550,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="187" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="187" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="187" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="187" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="187" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="187" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -578,20 +578,20 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="187" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="187" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="187" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="187" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="187" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="187" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -941,15 +941,15 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="18.69921875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="54.19921875" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="48" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:3" ht="48">
       <c r="A1" s="12" t="s">
         <v>32</v>
       </c>
@@ -960,7 +960,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -971,7 +971,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -982,7 +982,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="9" customFormat="1" ht="72">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -993,7 +993,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="8" spans="1:3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="9" spans="1:3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="13" spans="1:3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="14" spans="1:3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:3">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1123,7 +1123,7 @@
       </c>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:3">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1132,7 +1132,7 @@
       </c>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -1162,19 +1162,19 @@
       <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24"/>
   <cols>
     <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.86328125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.19921875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.69921875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="21.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:7" s="2" customFormat="1">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:7" s="2" customFormat="1">
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>184553</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:7" s="2" customFormat="1">
       <c r="A3" s="15" t="s">
         <v>4</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>217526</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:7" s="2" customFormat="1">
       <c r="A4" s="15" t="s">
         <v>5</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>208239</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:7" s="2" customFormat="1">
       <c r="A5" s="15" t="s">
         <v>6</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>153738</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:7" s="2" customFormat="1">
       <c r="A6" s="15" t="s">
         <v>7</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>175618</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:7" s="2" customFormat="1">
       <c r="A7" s="15" t="s">
         <v>12</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>173170</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="8" spans="1:7" s="2" customFormat="1">
       <c r="A8" s="15" t="s">
         <v>13</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>164107</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="9" spans="1:7" s="2" customFormat="1">
       <c r="A9" s="15" t="s">
         <v>14</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>162947</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:7" s="2" customFormat="1">
       <c r="A10" s="15" t="s">
         <v>15</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>175618</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:7" s="2" customFormat="1">
       <c r="A11" s="15" t="s">
         <v>16</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>195463</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:7" s="2" customFormat="1">
       <c r="A12" s="15" t="s">
         <v>17</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>179877</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="13" spans="1:7" s="2" customFormat="1">
       <c r="A13" s="15" t="s">
         <v>18</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>159610</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="14" spans="1:7">
       <c r="A14" s="15" t="s">
         <v>3</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>161695</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:7">
       <c r="A15" s="15" t="s">
         <v>4</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>195614</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:7">
       <c r="A16" s="15" t="s">
         <v>5</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>201277</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:7">
       <c r="A17" s="15" t="s">
         <v>6</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>154620</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:7">
       <c r="A18" s="15" t="s">
         <v>7</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>175689</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="19" spans="1:7">
       <c r="A19" s="15" t="s">
         <v>12</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>186616</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="20" spans="1:7">
       <c r="A20" s="15" t="s">
         <v>13</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>189967</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="21" spans="1:7">
       <c r="A21" s="15" t="s">
         <v>14</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>185940</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="22" spans="1:7">
       <c r="A22" s="15" t="s">
         <v>15</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>196229</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="23" spans="1:7">
       <c r="A23" s="15" t="s">
         <v>16</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>204397</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="24" spans="1:7">
       <c r="A24" s="15" t="s">
         <v>17</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>195666</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="25" spans="1:7">
       <c r="A25" s="15" t="s">
         <v>18</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>163065</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="26" spans="1:7">
       <c r="A26" s="15" t="s">
         <v>3</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>172693</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="27" spans="1:7">
       <c r="A27" s="15" t="s">
         <v>4</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>194813</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="28" spans="1:7">
       <c r="A28" s="15" t="s">
         <v>5</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>201224</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="29" spans="1:7">
       <c r="A29" s="15" t="s">
         <v>6</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>172071</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="30" spans="1:7">
       <c r="A30" s="15" t="s">
         <v>7</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>179195</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="31" spans="1:7">
       <c r="A31" s="15" t="s">
         <v>12</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>190551</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="32" spans="1:7">
       <c r="A32" s="15" t="s">
         <v>13</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>193433</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="33" spans="1:7">
       <c r="A33" s="15" t="s">
         <v>14</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>190539</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="34" spans="1:7">
       <c r="A34" s="15" t="s">
         <v>15</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>200583</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="35" spans="1:7">
       <c r="A35" s="15" t="s">
         <v>16</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>216782</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="36" spans="1:7">
       <c r="A36" s="15" t="s">
         <v>17</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>202539</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="37" spans="1:7">
       <c r="A37" s="15" t="s">
         <v>18</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>169754</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="38" spans="1:7">
       <c r="A38" s="15" t="s">
         <v>3</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>181895</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="39" spans="1:7">
       <c r="A39" s="15" t="s">
         <v>4</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>216976</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="40" spans="1:7">
       <c r="A40" s="15" t="s">
         <v>5</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>216976</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="41" spans="1:7">
       <c r="A41" s="15" t="s">
         <v>6</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>193129</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="42" spans="1:7">
       <c r="A42" s="15" t="s">
         <v>7</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>192124</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="43" spans="1:7">
       <c r="A43" s="15" t="s">
         <v>12</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>202362</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="44" spans="1:7">
       <c r="A44" s="15" t="s">
         <v>13</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>191479</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="45" spans="1:7">
       <c r="A45" s="15" t="s">
         <v>14</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>208325</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="46" spans="1:7">
       <c r="A46" s="15" t="s">
         <v>15</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>228210</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="47" spans="1:7">
       <c r="A47" s="15" t="s">
         <v>16</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>208345</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="48" spans="1:7">
       <c r="A48" s="15" t="s">
         <v>17</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>222752</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="49" spans="1:7">
       <c r="A49" s="15" t="s">
         <v>18</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>196821</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="50" spans="1:7">
       <c r="A50" s="15" t="s">
         <v>3</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>199724</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="51" spans="1:7">
       <c r="A51" s="15" t="s">
         <v>4</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>231754</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="52" spans="1:7">
       <c r="A52" s="15" t="s">
         <v>5</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>231483</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="53" spans="1:7">
       <c r="A53" s="15" t="s">
         <v>6</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>190772</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="54" spans="1:7">
       <c r="A54" s="15" t="s">
         <v>7</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>206662</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="55" spans="1:7">
       <c r="A55" s="15" t="s">
         <v>12</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>220220</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="56" spans="1:7">
       <c r="A56" s="15" t="s">
         <v>13</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>193037</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="57" spans="1:7">
       <c r="A57" s="15" t="s">
         <v>14</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>214320</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="58" spans="1:7">
       <c r="A58" s="15" t="s">
         <v>15</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>234453</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="59" spans="1:7">
       <c r="A59" s="15" t="s">
         <v>16</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>215490</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="60" spans="1:7">
       <c r="A60" s="15" t="s">
         <v>17</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>238568</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="61" spans="1:7">
       <c r="A61" s="15" t="s">
         <v>18</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>207004</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="62" spans="1:7">
       <c r="A62" s="15" t="s">
         <v>3</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>210419</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="63" spans="1:7">
       <c r="A63" s="15" t="s">
         <v>4</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>217720</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="64" spans="1:7">
       <c r="A64" s="15" t="s">
         <v>5</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>243464</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="65" spans="1:7">
       <c r="A65" s="15" t="s">
         <v>6</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>194589</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="66" spans="1:7">
       <c r="A66" s="15" t="s">
         <v>7</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>204743</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="67" spans="1:7">
       <c r="A67" s="15" t="s">
         <v>12</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>211106</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="68" spans="1:7">
       <c r="A68" s="15" t="s">
         <v>13</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>217778</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="69" spans="1:7">
       <c r="A69" s="15" t="s">
         <v>14</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>255228</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="70" spans="1:7">
       <c r="A70" s="15" t="s">
         <v>15</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>285215</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="71" spans="1:7">
       <c r="A71" s="15" t="s">
         <v>16</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>262674</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="72" spans="1:7">
       <c r="A72" s="15" t="s">
         <v>17</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>332185</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="73" spans="1:7">
       <c r="A73" s="15" t="s">
         <v>18</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>279842</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="74" spans="1:7">
       <c r="A74" s="15" t="s">
         <v>3</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>288295</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="75" spans="1:7">
       <c r="A75" s="15" t="s">
         <v>4</v>
       </c>
@@ -2899,7 +2899,7 @@
         <v>251046</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="76" spans="1:7">
       <c r="A76" s="15" t="s">
         <v>5</v>
       </c>
@@ -2922,7 +2922,7 @@
         <v>128090</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="77" spans="1:7">
       <c r="A77" s="15" t="s">
         <v>6</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>34468</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="78" spans="1:7">
       <c r="A78" s="15" t="s">
         <v>7</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>74876</v>
       </c>
     </row>
-    <row r="79" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="79" spans="1:7" s="32" customFormat="1">
       <c r="A79" s="15" t="s">
         <v>12</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>133543</v>
       </c>
     </row>
-    <row r="80" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="80" spans="1:7" s="32" customFormat="1">
       <c r="A80" s="15" t="s">
         <v>13</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>168094</v>
       </c>
     </row>
-    <row r="81" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="81" spans="1:7" s="32" customFormat="1">
       <c r="A81" s="15" t="s">
         <v>14</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>190764</v>
       </c>
     </row>
-    <row r="82" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="82" spans="1:7" s="32" customFormat="1">
       <c r="A82" s="15" t="s">
         <v>15</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>199061</v>
       </c>
     </row>
-    <row r="83" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="83" spans="1:7" s="32" customFormat="1">
       <c r="A83" s="15" t="s">
         <v>16</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>176109</v>
       </c>
     </row>
-    <row r="84" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="84" spans="1:7" s="32" customFormat="1">
       <c r="A84" s="24" t="s">
         <v>17</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>223167</v>
       </c>
     </row>
-    <row r="85" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="85" spans="1:7" s="32" customFormat="1">
       <c r="A85" s="24" t="s">
         <v>18</v>
       </c>
@@ -3129,13 +3129,13 @@
         <v>179124</v>
       </c>
     </row>
-    <row r="132" s="32" customFormat="1" x14ac:dyDescent="0.65"/>
-    <row r="133" s="32" customFormat="1" x14ac:dyDescent="0.65"/>
-    <row r="134" s="32" customFormat="1" x14ac:dyDescent="0.65"/>
-    <row r="135" s="32" customFormat="1" x14ac:dyDescent="0.65"/>
-    <row r="136" s="32" customFormat="1" x14ac:dyDescent="0.65"/>
-    <row r="137" s="32" customFormat="1" x14ac:dyDescent="0.65"/>
-    <row r="138" s="32" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="132" s="32" customFormat="1"/>
+    <row r="133" s="32" customFormat="1"/>
+    <row r="134" s="32" customFormat="1"/>
+    <row r="135" s="32" customFormat="1"/>
+    <row r="136" s="32" customFormat="1"/>
+    <row r="137" s="32" customFormat="1"/>
+    <row r="138" s="32" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="89" orientation="landscape" r:id="rId1"/>
@@ -3147,20 +3147,21 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="4.8984375" customWidth="1"/>
+    <col min="1" max="1" width="18.73046875" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
     <col min="3" max="3" width="32.59765625" customWidth="1"/>
-    <col min="4" max="4" width="17.09765625" customWidth="1"/>
+    <col min="4" max="4" width="17.06640625" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="28.69921875" customWidth="1"/>
-    <col min="7" max="7" width="26.09765625" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" customWidth="1"/>
+    <col min="7" max="7" width="26.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:7" ht="24">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3183,7 +3184,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:7" ht="24">
       <c r="A2" s="15" t="s">
         <v>14</v>
       </c>
@@ -3206,7 +3207,7 @@
         <v>19568</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:7" ht="24">
       <c r="A3" s="15" t="s">
         <v>15</v>
       </c>
@@ -3229,7 +3230,7 @@
         <v>16437</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:7" ht="24">
       <c r="A4" s="15" t="s">
         <v>16</v>
       </c>
@@ -3252,7 +3253,7 @@
         <v>15140</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:7" ht="24">
       <c r="A5" s="15" t="s">
         <v>17</v>
       </c>
@@ -3275,7 +3276,7 @@
         <v>14264</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:7" ht="24">
       <c r="A6" s="15" t="s">
         <v>18</v>
       </c>
@@ -3298,7 +3299,7 @@
         <v>12093</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:7" ht="24">
       <c r="A7" s="15" t="s">
         <v>3</v>
       </c>
@@ -3321,7 +3322,7 @@
         <v>13538</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="8" spans="1:7" ht="24">
       <c r="A8" s="15" t="s">
         <v>4</v>
       </c>
@@ -3344,7 +3345,7 @@
         <v>14248</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="9" spans="1:7" ht="24">
       <c r="A9" s="15" t="s">
         <v>5</v>
       </c>
@@ -3367,7 +3368,7 @@
         <v>16741</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:7" ht="24">
       <c r="A10" s="15" t="s">
         <v>6</v>
       </c>
@@ -3390,7 +3391,7 @@
         <v>15750</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:7" ht="24">
       <c r="A11" s="15" t="s">
         <v>7</v>
       </c>
@@ -3413,7 +3414,7 @@
         <v>16901</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:7" ht="24">
       <c r="A12" s="15" t="s">
         <v>12</v>
       </c>
@@ -3436,7 +3437,7 @@
         <v>19066</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="13" spans="1:7" ht="24">
       <c r="A13" s="15" t="s">
         <v>13</v>
       </c>
@@ -3459,7 +3460,7 @@
         <v>18749</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="14" spans="1:7" ht="24">
       <c r="A14" s="15" t="s">
         <v>14</v>
       </c>
@@ -3482,7 +3483,7 @@
         <v>28436</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:7" ht="24">
       <c r="A15" s="15" t="s">
         <v>15</v>
       </c>
@@ -3505,7 +3506,7 @@
         <v>34278</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:7" ht="24">
       <c r="A16" s="15" t="s">
         <v>16</v>
       </c>
@@ -3528,7 +3529,7 @@
         <v>32140</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:7" ht="24">
       <c r="A17" s="15" t="s">
         <v>17</v>
       </c>
@@ -3551,7 +3552,7 @@
         <v>31330</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:7" ht="24">
       <c r="A18" s="15" t="s">
         <v>18</v>
       </c>
@@ -3574,7 +3575,7 @@
         <v>27470</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="19" spans="1:7" ht="24">
       <c r="A19" s="15" t="s">
         <v>3</v>
       </c>
@@ -3597,7 +3598,7 @@
         <v>27495</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="20" spans="1:7" ht="24">
       <c r="A20" s="15" t="s">
         <v>4</v>
       </c>
@@ -3620,7 +3621,7 @@
         <v>29846</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="21" spans="1:7" ht="24">
       <c r="A21" s="15" t="s">
         <v>5</v>
       </c>
@@ -3643,7 +3644,7 @@
         <v>30877</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="22" spans="1:7" ht="24">
       <c r="A22" s="15" t="s">
         <v>6</v>
       </c>
@@ -3666,7 +3667,7 @@
         <v>26756</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="23" spans="1:7" ht="24">
       <c r="A23" s="15" t="s">
         <v>7</v>
       </c>
@@ -3689,7 +3690,7 @@
         <v>30412</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="24" spans="1:7" ht="24">
       <c r="A24" s="15" t="s">
         <v>12</v>
       </c>
@@ -3712,7 +3713,7 @@
         <v>33341</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="25" spans="1:7" ht="24">
       <c r="A25" s="15" t="s">
         <v>13</v>
       </c>
@@ -3735,7 +3736,7 @@
         <v>30199</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="26" spans="1:7" ht="24">
       <c r="A26" s="15" t="s">
         <v>14</v>
       </c>
@@ -3758,7 +3759,7 @@
         <v>33034</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="27" spans="1:7" ht="24">
       <c r="A27" s="15" t="s">
         <v>15</v>
       </c>
@@ -3781,7 +3782,7 @@
         <v>35653</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="28" spans="1:7" ht="24">
       <c r="A28" s="15" t="s">
         <v>16</v>
       </c>
@@ -3804,7 +3805,7 @@
         <v>32414</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="29" spans="1:7" ht="24">
       <c r="A29" s="15" t="s">
         <v>17</v>
       </c>
@@ -3827,7 +3828,7 @@
         <v>36004</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="30" spans="1:7" ht="24">
       <c r="A30" s="15" t="s">
         <v>18</v>
       </c>
@@ -3850,7 +3851,7 @@
         <v>33624</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="31" spans="1:7" ht="24">
       <c r="A31" s="15" t="s">
         <v>3</v>
       </c>
@@ -3873,7 +3874,7 @@
         <v>32252</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="32" spans="1:7" ht="24">
       <c r="A32" s="15" t="s">
         <v>4</v>
       </c>
@@ -3896,7 +3897,7 @@
         <v>32967</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="33" spans="1:7" ht="24">
       <c r="A33" s="15" t="s">
         <v>5</v>
       </c>
@@ -3919,7 +3920,7 @@
         <v>37284</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="34" spans="1:7" ht="24">
       <c r="A34" s="15" t="s">
         <v>6</v>
       </c>
@@ -3942,7 +3943,7 @@
         <v>30052</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="35" spans="1:7" ht="24">
       <c r="A35" s="15" t="s">
         <v>7</v>
       </c>
@@ -3965,7 +3966,7 @@
         <v>34177</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="36" spans="1:7" ht="24">
       <c r="A36" s="15" t="s">
         <v>12</v>
       </c>
@@ -3988,7 +3989,7 @@
         <v>36112</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="37" spans="1:7" ht="24">
       <c r="A37" s="15" t="s">
         <v>13</v>
       </c>
@@ -4011,7 +4012,7 @@
         <v>35601</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="38" spans="1:7" ht="24">
       <c r="A38" s="15" t="s">
         <v>14</v>
       </c>
@@ -4034,7 +4035,7 @@
         <v>36039</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="39" spans="1:7" ht="24">
       <c r="A39" s="15" t="s">
         <v>15</v>
       </c>
@@ -4057,7 +4058,7 @@
         <v>36468</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="40" spans="1:7" ht="24">
       <c r="A40" s="15" t="s">
         <v>16</v>
       </c>
@@ -4080,7 +4081,7 @@
         <v>35614</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="41" spans="1:7" ht="24">
       <c r="A41" s="15" t="s">
         <v>17</v>
       </c>
@@ -4103,7 +4104,7 @@
         <v>42910</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="42" spans="1:7" ht="24">
       <c r="A42" s="15" t="s">
         <v>18</v>
       </c>
@@ -4126,7 +4127,7 @@
         <v>35783</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="43" spans="1:7" ht="24">
       <c r="A43" s="15" t="s">
         <v>3</v>
       </c>
@@ -4149,7 +4150,7 @@
         <v>37401</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="44" spans="1:7" ht="24">
       <c r="A44" s="15" t="s">
         <v>4</v>
       </c>
@@ -4172,7 +4173,7 @@
         <v>36442</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="45" spans="1:7" ht="24">
       <c r="A45" s="15" t="s">
         <v>5</v>
       </c>
@@ -4195,7 +4196,7 @@
         <v>20450</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="46" spans="1:7" ht="24">
       <c r="A46" s="15" t="s">
         <v>6</v>
       </c>
@@ -4218,7 +4219,7 @@
         <v>6797</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="47" spans="1:7" ht="24">
       <c r="A47" s="15" t="s">
         <v>7</v>
       </c>
@@ -4241,7 +4242,7 @@
         <v>14167</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="48" spans="1:7" ht="24">
       <c r="A48" s="15" t="s">
         <v>12</v>
       </c>
@@ -4264,7 +4265,7 @@
         <v>24320</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="49" spans="1:7" ht="24">
       <c r="A49" s="15" t="s">
         <v>13</v>
       </c>
@@ -4287,7 +4288,7 @@
         <v>29882</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="50" spans="1:7" ht="24">
       <c r="A50" s="15" t="s">
         <v>14</v>
       </c>
@@ -4310,7 +4311,7 @@
         <v>33419</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="51" spans="1:7" ht="24">
       <c r="A51" s="15" t="s">
         <v>15</v>
       </c>
@@ -4333,7 +4334,7 @@
         <v>35228</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="52" spans="1:7" ht="24">
       <c r="A52" s="15" t="s">
         <v>16</v>
       </c>
@@ -4356,7 +4357,7 @@
         <v>32882</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="53" spans="1:7" ht="24">
       <c r="A53" s="24" t="s">
         <v>17</v>
       </c>
@@ -4379,7 +4380,7 @@
         <v>39956</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="24" x14ac:dyDescent="0.65">
+    <row r="54" spans="1:7" ht="24">
       <c r="A54" s="24" t="s">
         <v>18</v>
       </c>

</xml_diff>